<commit_message>
load check in massive conversion main
</commit_message>
<xml_diff>
--- a/asignaciones.xlsx
+++ b/asignaciones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\f-sigebi2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\f-sigebi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635EF50D-8FEA-4077-90ED-03E21C59D4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B984091-C56C-4983-8779-9875216FD35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BF87A032-DF41-4815-8520-0592C1777C61}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF87A032-DF41-4815-8520-0592C1777C61}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -282,7 +282,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -754,10 +754,10 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="21.44140625" customWidth="1"/>
     <col min="2" max="2" width="33.109375" customWidth="1"/>
@@ -768,7 +768,7 @@
     <col min="7" max="7" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="16.2" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -788,7 +788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="10" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="10" customFormat="1" ht="21" thickBot="1">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -810,7 +810,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="1:8" s="10" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="10" customFormat="1" ht="21" thickBot="1">
       <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
@@ -832,7 +832,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:8" s="10" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="10" customFormat="1" ht="21" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
@@ -854,7 +854,7 @@
       <c r="G4" s="8"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="10" customFormat="1" ht="21" thickBot="1">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -875,7 +875,7 @@
       </c>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="21" thickBot="1">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -896,7 +896,7 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" ht="51.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="4" customFormat="1" ht="51.6" thickBot="1">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -920,8 +920,8 @@
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="13" customFormat="1" ht="15" thickBot="1"/>
+    <row r="9" spans="1:8" ht="21" thickBot="1">
       <c r="A9" s="12" t="s">
         <v>35</v>
       </c>
@@ -938,7 +938,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="21" thickBot="1">
       <c r="A10" s="12" t="s">
         <v>38</v>
       </c>
@@ -961,7 +961,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="18" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" s="18" customFormat="1" ht="21" thickBot="1">
       <c r="A11" s="15" t="s">
         <v>43</v>
       </c>
@@ -981,7 +981,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="31.2" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>47</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="21" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>49</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="31.2" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>51</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="31.2" thickBot="1">
       <c r="A15" s="12" t="s">
         <v>53</v>
       </c>
@@ -1065,15 +1065,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010039E1E462ED92E146BDA8C6EE3E6510EA" ma:contentTypeVersion="7" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="8c7358d94f38434d930b304687946edc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c0a1bb40-100d-482c-9e92-ade20f327aab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="495aae5eb407c7acbb2fa756d4a0460a" ns3:_="">
     <xsd:import namespace="c0a1bb40-100d-482c-9e92-ade20f327aab"/>
@@ -1237,6 +1228,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1244,14 +1244,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EF63720-6B71-41F1-9DDE-C7BAD8E96D3D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13EFFB92-C78B-4A5A-8992-27FE58E33A8C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1265,6 +1257,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EF63720-6B71-41F1-9DDE-C7BAD8E96D3D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>